<commit_message>
Adding passive and attack data reading
</commit_message>
<xml_diff>
--- a/ProjectApopalypse_Unity/Excel/Units.xlsx
+++ b/ProjectApopalypse_Unity/Excel/Units.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectApopalypse\ProjectApopalypse_Unity\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BDFC50-205E-4320-A9D8-2220438703C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8523B34C-C01D-4B21-A3E4-07A1626A11A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{3A2312A1-F630-46F4-AF7A-37D6220B2126}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="87">
   <si>
     <t>technicalName</t>
   </si>
@@ -258,9 +258,6 @@
     <t>attack4</t>
   </si>
   <si>
-    <t>attack5</t>
-  </si>
-  <si>
     <t>lorenzo</t>
   </si>
   <si>
@@ -285,10 +282,10 @@
     <t>passive4</t>
   </si>
   <si>
-    <t>passive5</t>
-  </si>
-  <si>
     <t>defaultPassive</t>
+  </si>
+  <si>
+    <t>basicAttack</t>
   </si>
 </sst>
 </file>
@@ -648,21 +645,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66FF625-BC64-4C5F-8916-6942D597EF48}">
-  <dimension ref="A1:CB4"/>
+  <dimension ref="A1:CA4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="7.8" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8.33203125" style="1" customWidth="1"/>
-    <col min="2" max="12" width="8.77734375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="8.88671875" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="1"/>
+    <col min="2" max="11" width="8.77734375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:80" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:79" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -670,241 +667,238 @@
         <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="H1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>86</v>
+        <v>1</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>38</v>
+        <v>2</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AZ1" s="1" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="BA1" s="1" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="BB1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="BE1" s="1" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="BF1" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="BG1" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="BH1" s="1" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="BI1" s="1" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="BJ1" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="BK1" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="BL1" s="1" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="BM1" s="1" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="BN1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="BO1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="BP1" s="1" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="BQ1" s="1" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="BR1" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="BS1" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="BT1" s="1" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="BU1" s="1" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="BV1" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="BW1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="BX1" s="1" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="BY1" s="1" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="BZ1" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="CA1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="CB1" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:80" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:79" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -914,217 +908,220 @@
       <c r="C2" s="1" t="s">
         <v>72</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L2" s="1">
+        <v>10</v>
+      </c>
       <c r="M2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="N2" s="1">
-        <v>999</v>
-      </c>
-      <c r="O2" s="1">
-        <v>1</v>
-      </c>
-      <c r="P2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="O2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="P2" s="1">
+        <v>10</v>
       </c>
       <c r="Q2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="R2" s="1">
-        <v>999</v>
-      </c>
-      <c r="S2" s="1">
-        <v>1</v>
-      </c>
-      <c r="T2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="S2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1">
+        <v>10</v>
       </c>
       <c r="U2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="V2" s="1">
-        <v>999</v>
-      </c>
-      <c r="W2" s="1">
-        <v>1</v>
-      </c>
-      <c r="X2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="W2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="X2" s="1">
+        <v>10</v>
       </c>
       <c r="Y2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="Z2" s="1">
-        <v>999</v>
-      </c>
-      <c r="AA2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AB2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AA2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>10</v>
       </c>
       <c r="AC2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="AD2" s="1">
-        <v>999</v>
-      </c>
-      <c r="AE2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AF2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AE2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>10</v>
       </c>
       <c r="AG2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="AH2" s="1">
-        <v>999</v>
-      </c>
-      <c r="AI2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AJ2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AI2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>10</v>
       </c>
       <c r="AK2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="AL2" s="1">
-        <v>999</v>
-      </c>
-      <c r="AM2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AN2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AM2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN2" s="1">
+        <v>10</v>
       </c>
       <c r="AO2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="AP2" s="1">
-        <v>999</v>
-      </c>
-      <c r="AQ2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AR2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AQ2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR2" s="1">
+        <v>10</v>
       </c>
       <c r="AS2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="AT2" s="1">
-        <v>999</v>
-      </c>
-      <c r="AU2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AV2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AU2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV2" s="1">
+        <v>10</v>
       </c>
       <c r="AW2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="AX2" s="1">
-        <v>999</v>
-      </c>
-      <c r="AY2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AZ2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AY2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AZ2" s="1">
+        <v>10</v>
       </c>
       <c r="BA2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="BB2" s="1">
-        <v>999</v>
-      </c>
-      <c r="BC2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BD2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="BC2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BD2" s="1">
+        <v>10</v>
       </c>
       <c r="BE2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="BF2" s="1">
-        <v>999</v>
-      </c>
-      <c r="BG2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BH2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="BG2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BH2" s="1">
+        <v>10</v>
       </c>
       <c r="BI2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="BJ2" s="1">
-        <v>999</v>
-      </c>
-      <c r="BK2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BL2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="BK2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BL2" s="1">
+        <v>10</v>
       </c>
       <c r="BM2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="BN2" s="1">
-        <v>999</v>
-      </c>
-      <c r="BO2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BP2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="BO2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BP2" s="1">
+        <v>10</v>
       </c>
       <c r="BQ2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="BR2" s="1">
-        <v>999</v>
-      </c>
-      <c r="BS2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BT2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="BS2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BT2" s="1">
+        <v>10</v>
       </c>
       <c r="BU2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="BV2" s="1">
-        <v>999</v>
-      </c>
-      <c r="BW2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BX2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="BW2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BX2" s="1">
+        <v>10</v>
       </c>
       <c r="BY2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="BZ2" s="1">
-        <v>999</v>
-      </c>
-      <c r="CA2" s="1">
-        <v>1</v>
-      </c>
-      <c r="CB2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="CA2" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:80" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:79" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>72</v>
@@ -1135,60 +1132,60 @@
       <c r="E3" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="G3" s="1" t="s">
         <v>72</v>
       </c>
+      <c r="H3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L3" s="1">
+        <v>500</v>
+      </c>
       <c r="M3" s="1">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="N3" s="1">
-        <v>700</v>
-      </c>
-      <c r="O3" s="1">
-        <v>1</v>
-      </c>
-      <c r="P3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:80" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:79" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>72</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
+      </c>
+      <c r="L4" s="1">
+        <v>25</v>
       </c>
       <c r="M4" s="1">
-        <v>25</v>
+        <v>500</v>
       </c>
       <c r="N4" s="1">
-        <v>500</v>
-      </c>
-      <c r="O4" s="1">
         <v>5</v>
       </c>
-      <c r="P4" s="1" t="b">
-        <v>0</v>
+      <c r="O4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1">
+        <v>5</v>
       </c>
       <c r="Q4" s="1">
+        <v>999</v>
+      </c>
+      <c r="R4" s="1">
         <v>5</v>
       </c>
-      <c r="R4" s="1">
-        <v>999</v>
-      </c>
-      <c r="S4" s="1">
-        <v>5</v>
-      </c>
-      <c r="T4" s="1" t="b">
+      <c r="S4" s="1" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding set current variables functionality
</commit_message>
<xml_diff>
--- a/ProjectApopalypse_Unity/Excel/Units.xlsx
+++ b/ProjectApopalypse_Unity/Excel/Units.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectApopalypse\ProjectApopalypse_Unity\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BDC0C71-56CA-433A-8B02-A153210E5A27}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C271BB41-A0C8-4FE9-82D5-119690643239}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{3A2312A1-F630-46F4-AF7A-37D6220B2126}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
   <si>
     <t>technicalName</t>
   </si>
@@ -243,9 +243,6 @@
     <t>actMoveSpeedLocked</t>
   </si>
   <si>
-    <t>defaultAttack</t>
-  </si>
-  <si>
     <t>passive1</t>
   </si>
   <si>
@@ -261,9 +258,6 @@
     <t>defaultPassive</t>
   </si>
   <si>
-    <t>basicAttack</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -273,9 +267,6 @@
     <t>attackType</t>
   </si>
   <si>
-    <t>Melee</t>
-  </si>
-  <si>
     <t>actCharges</t>
   </si>
   <si>
@@ -298,6 +289,27 @@
   </si>
   <si>
     <t>actSalvoLocked</t>
+  </si>
+  <si>
+    <t>canMove</t>
+  </si>
+  <si>
+    <t>moveType</t>
+  </si>
+  <si>
+    <t>canAttack</t>
+  </si>
+  <si>
+    <t>Flying</t>
+  </si>
+  <si>
+    <t>Ranged</t>
+  </si>
+  <si>
+    <t>rank</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -657,21 +669,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66FF625-BC64-4C5F-8916-6942D597EF48}">
-  <dimension ref="A1:CG2"/>
+  <dimension ref="A1:CJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BK1" workbookViewId="0">
-      <selection activeCell="CG1" sqref="CG1"/>
+    <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
+      <selection activeCell="BI3" sqref="BI3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="7.8" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8.33203125" style="1" customWidth="1"/>
-    <col min="2" max="9" width="8.77734375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="1"/>
+    <col min="2" max="12" width="8.77734375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="8.88671875" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:88" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -679,256 +691,265 @@
         <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BS1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BT1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BU1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BW1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="BX1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BY1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="BZ1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="CA1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="CB1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="CC1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="CD1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="BB1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="BD1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="BE1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="BF1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="BG1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="BH1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="BI1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="BJ1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="BK1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="BL1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="BM1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="BN1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="BO1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="BP1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="BQ1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="BR1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BS1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="BT1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="BU1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="BV1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="BW1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BX1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="BY1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="BZ1" s="1" t="s">
+      <c r="CE1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="CF1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="CA1" s="1" t="s">
+      <c r="CG1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="CB1" s="1" t="s">
+      <c r="CH1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="CC1" s="1" t="s">
+      <c r="CI1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="CD1" s="1" t="s">
+      <c r="CJ1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="CE1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="CF1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="CG1" s="1" t="s">
-        <v>90</v>
-      </c>
     </row>
-    <row r="2" spans="1:85" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:88" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -936,243 +957,252 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="J2" s="1">
-        <v>10</v>
-      </c>
-      <c r="K2" s="1">
-        <v>999</v>
-      </c>
-      <c r="L2" s="1">
-        <v>1</v>
-      </c>
-      <c r="M2" s="1" t="b">
-        <v>0</v>
+        <v>94</v>
+      </c>
+      <c r="E2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M2" s="1">
+        <v>10</v>
       </c>
       <c r="N2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="O2" s="1">
-        <v>999</v>
-      </c>
-      <c r="P2" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="P2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>10</v>
       </c>
       <c r="R2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="S2" s="1">
-        <v>999</v>
-      </c>
-      <c r="T2" s="1">
-        <v>1</v>
-      </c>
-      <c r="U2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="T2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="U2" s="1">
+        <v>10</v>
       </c>
       <c r="V2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="W2" s="1">
-        <v>999</v>
-      </c>
-      <c r="X2" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="X2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>10</v>
       </c>
       <c r="Z2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="AA2" s="1">
-        <v>999</v>
-      </c>
-      <c r="AB2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AC2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AB2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>10</v>
       </c>
       <c r="AD2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="AE2" s="1">
-        <v>999</v>
-      </c>
-      <c r="AF2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AG2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AF2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>10</v>
       </c>
       <c r="AH2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="AI2" s="1">
-        <v>999</v>
-      </c>
-      <c r="AJ2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AK2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="1">
+        <v>10</v>
       </c>
       <c r="AL2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="AM2" s="1">
-        <v>999</v>
-      </c>
-      <c r="AN2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AO2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AN2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO2" s="1">
+        <v>10</v>
       </c>
       <c r="AP2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="AQ2" s="1">
-        <v>999</v>
-      </c>
-      <c r="AR2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AS2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AR2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS2" s="1">
+        <v>10</v>
       </c>
       <c r="AT2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="AU2" s="1">
-        <v>999</v>
-      </c>
-      <c r="AV2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AW2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AV2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AW2" s="1">
+        <v>10</v>
       </c>
       <c r="AX2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="AY2" s="1">
-        <v>999</v>
-      </c>
-      <c r="AZ2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BA2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AZ2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BA2" s="1">
+        <v>10</v>
       </c>
       <c r="BB2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="BC2" s="1">
-        <v>999</v>
-      </c>
-      <c r="BD2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BE2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="BD2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BE2" s="1">
+        <v>10</v>
       </c>
       <c r="BF2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="BG2" s="1">
-        <v>999</v>
-      </c>
-      <c r="BH2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BI2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="BH2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BI2" s="1">
+        <v>2</v>
       </c>
       <c r="BJ2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="BK2" s="1">
-        <v>999</v>
-      </c>
-      <c r="BL2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BM2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="BL2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BM2" s="1">
+        <v>10</v>
       </c>
       <c r="BN2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="BO2" s="1">
-        <v>999</v>
-      </c>
-      <c r="BP2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BQ2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="BP2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BQ2" s="1">
+        <v>10</v>
       </c>
       <c r="BR2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="BS2" s="1">
-        <v>999</v>
-      </c>
-      <c r="BT2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BU2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="BT2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BU2" s="1">
+        <v>10</v>
       </c>
       <c r="BV2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="BW2" s="1">
-        <v>999</v>
-      </c>
-      <c r="BX2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BY2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="BX2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BY2" s="1">
+        <v>10</v>
       </c>
       <c r="BZ2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="CA2" s="1">
-        <v>999</v>
-      </c>
-      <c r="CB2" s="1">
-        <v>1</v>
-      </c>
-      <c r="CC2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="CB2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="CC2" s="1">
+        <v>10</v>
       </c>
       <c r="CD2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="CE2" s="1">
-        <v>999</v>
-      </c>
-      <c r="CF2" s="1">
-        <v>1</v>
-      </c>
-      <c r="CG2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="CF2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="CG2" s="1">
+        <v>10</v>
+      </c>
+      <c r="CH2" s="1">
+        <v>999</v>
+      </c>
+      <c r="CI2" s="1">
+        <v>1</v>
+      </c>
+      <c r="CJ2" s="1" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Working on attack functionality
</commit_message>
<xml_diff>
--- a/ProjectApopalypse_Unity/Excel/Units.xlsx
+++ b/ProjectApopalypse_Unity/Excel/Units.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectApopalypse\ProjectApopalypse_Unity\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C271BB41-A0C8-4FE9-82D5-119690643239}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC96B6AE-19BB-4E28-BF01-7E844E746FF4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{3A2312A1-F630-46F4-AF7A-37D6220B2126}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
   <si>
     <t>technicalName</t>
   </si>
@@ -264,9 +264,6 @@
     <t>This is the default unit. The genesis of all life. Where all life derives.</t>
   </si>
   <si>
-    <t>attackType</t>
-  </si>
-  <si>
     <t>actCharges</t>
   </si>
   <si>
@@ -303,13 +300,37 @@
     <t>Flying</t>
   </si>
   <si>
-    <t>Ranged</t>
-  </si>
-  <si>
     <t>rank</t>
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>splashType</t>
+  </si>
+  <si>
+    <t>attackOrigin</t>
+  </si>
+  <si>
+    <t>Targets</t>
+  </si>
+  <si>
+    <t>Sphere</t>
+  </si>
+  <si>
+    <t>actTargets</t>
+  </si>
+  <si>
+    <t>actTargetsMax</t>
+  </si>
+  <si>
+    <t>actTargetsMin</t>
+  </si>
+  <si>
+    <t>actTargetsLocked</t>
+  </si>
+  <si>
+    <t>salvoRate</t>
   </si>
 </sst>
 </file>
@@ -669,21 +690,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66FF625-BC64-4C5F-8916-6942D597EF48}">
-  <dimension ref="A1:CJ2"/>
+  <dimension ref="A1:CP2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
-      <selection activeCell="BI3" sqref="BI3"/>
+    <sheetView tabSelected="1" topLeftCell="BS1" workbookViewId="0">
+      <selection activeCell="CL2" sqref="CL2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="7.8" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8.33203125" style="1" customWidth="1"/>
-    <col min="2" max="12" width="8.77734375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="8.88671875" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="1"/>
+    <col min="2" max="13" width="8.77734375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="8.88671875" style="1" customWidth="1"/>
+    <col min="15" max="88" width="8.88671875" style="1"/>
+    <col min="89" max="90" width="9.21875" style="1" customWidth="1"/>
+    <col min="91" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:94" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -694,262 +717,280 @@
         <v>77</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="BS1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BT1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BU1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BW1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BX1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="BY1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BZ1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="CA1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="CB1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="CC1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="CD1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="BB1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="BD1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="BE1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="BF1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="BG1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="BH1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="BI1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="BJ1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="BK1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="BL1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="BM1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="BN1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="BO1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="BP1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="BQ1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="BR1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="BS1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="BT1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="BU1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BV1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="BW1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="BX1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="BY1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="BZ1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="CA1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="CB1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="CC1" s="1" t="s">
+      <c r="CE1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="CD1" s="1" t="s">
+      <c r="CF1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="CE1" s="1" t="s">
+      <c r="CG1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="CF1" s="1" t="s">
+      <c r="CH1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="CG1" s="1" t="s">
+      <c r="CI1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="CH1" s="1" t="s">
+      <c r="CJ1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="CI1" s="1" t="s">
+      <c r="CK1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="CJ1" s="1" t="s">
-        <v>87</v>
+      <c r="CL1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="CM1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="CN1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="CO1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="CP1" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:94" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -960,7 +1001,7 @@
         <v>78</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E2" s="1" t="b">
         <v>1</v>
@@ -969,240 +1010,258 @@
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="M2" s="1">
-        <v>10</v>
-      </c>
       <c r="N2" s="1">
-        <v>999</v>
+        <v>10</v>
       </c>
       <c r="O2" s="1">
-        <v>1</v>
-      </c>
-      <c r="P2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>10</v>
+        <v>999</v>
+      </c>
+      <c r="P2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="R2" s="1">
-        <v>999</v>
+        <v>10</v>
       </c>
       <c r="S2" s="1">
-        <v>1</v>
-      </c>
-      <c r="T2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="U2" s="1">
-        <v>10</v>
+        <v>999</v>
+      </c>
+      <c r="T2" s="1">
+        <v>1</v>
+      </c>
+      <c r="U2" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="V2" s="1">
-        <v>999</v>
+        <v>10</v>
       </c>
       <c r="W2" s="1">
-        <v>1</v>
-      </c>
-      <c r="X2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="1">
-        <v>10</v>
+        <v>999</v>
+      </c>
+      <c r="X2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="Z2" s="1">
-        <v>999</v>
+        <v>10</v>
       </c>
       <c r="AA2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AB2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="1">
-        <v>10</v>
+        <v>999</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="AD2" s="1">
-        <v>999</v>
+        <v>10</v>
       </c>
       <c r="AE2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AF2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG2" s="1">
-        <v>10</v>
+        <v>999</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="AH2" s="1">
-        <v>999</v>
+        <v>10</v>
       </c>
       <c r="AI2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AJ2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="AK2" s="1">
-        <v>10</v>
+        <v>999</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK2" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="AL2" s="1">
-        <v>999</v>
+        <v>10</v>
       </c>
       <c r="AM2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AN2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="AO2" s="1">
-        <v>10</v>
+        <v>999</v>
+      </c>
+      <c r="AN2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AO2" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="AP2" s="1">
-        <v>999</v>
+        <v>10</v>
       </c>
       <c r="AQ2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AR2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="AS2" s="1">
-        <v>10</v>
+        <v>999</v>
+      </c>
+      <c r="AR2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS2" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="AT2" s="1">
-        <v>999</v>
+        <v>10</v>
       </c>
       <c r="AU2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AV2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="AW2" s="1">
-        <v>10</v>
+        <v>999</v>
+      </c>
+      <c r="AV2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW2" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="AX2" s="1">
-        <v>999</v>
+        <v>10</v>
       </c>
       <c r="AY2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AZ2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="BA2" s="1">
-        <v>10</v>
+        <v>999</v>
+      </c>
+      <c r="AZ2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BA2" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="BB2" s="1">
-        <v>999</v>
+        <v>10</v>
       </c>
       <c r="BC2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BD2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="BE2" s="1">
-        <v>10</v>
+        <v>999</v>
+      </c>
+      <c r="BD2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BE2" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="BF2" s="1">
-        <v>999</v>
+        <v>10</v>
       </c>
       <c r="BG2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BH2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="BI2" s="1">
+        <v>999</v>
+      </c>
+      <c r="BH2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BI2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BJ2" s="1">
         <v>2</v>
       </c>
-      <c r="BJ2" s="1">
-        <v>999</v>
-      </c>
       <c r="BK2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BL2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="BM2" s="1">
-        <v>10</v>
+        <v>999</v>
+      </c>
+      <c r="BL2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BM2" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="BN2" s="1">
-        <v>999</v>
+        <v>1</v>
       </c>
       <c r="BO2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BP2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="BQ2" s="1">
-        <v>10</v>
+        <v>999</v>
+      </c>
+      <c r="BP2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BQ2" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="BR2" s="1">
-        <v>999</v>
+        <v>10</v>
       </c>
       <c r="BS2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BT2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="BU2" s="1">
-        <v>10</v>
+        <v>999</v>
+      </c>
+      <c r="BT2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BU2" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="BV2" s="1">
-        <v>999</v>
+        <v>10</v>
       </c>
       <c r="BW2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BX2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="BY2" s="1">
-        <v>10</v>
+        <v>999</v>
+      </c>
+      <c r="BX2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BY2" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="BZ2" s="1">
-        <v>999</v>
+        <v>10</v>
       </c>
       <c r="CA2" s="1">
-        <v>1</v>
-      </c>
-      <c r="CB2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="CC2" s="1">
-        <v>10</v>
+        <v>999</v>
+      </c>
+      <c r="CB2" s="1">
+        <v>1</v>
+      </c>
+      <c r="CC2" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="CD2" s="1">
-        <v>999</v>
+        <v>10</v>
       </c>
       <c r="CE2" s="1">
-        <v>1</v>
-      </c>
-      <c r="CF2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="CG2" s="1">
-        <v>10</v>
+        <v>999</v>
+      </c>
+      <c r="CF2" s="1">
+        <v>1</v>
+      </c>
+      <c r="CG2" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="CH2" s="1">
-        <v>999</v>
+        <v>10</v>
       </c>
       <c r="CI2" s="1">
-        <v>1</v>
-      </c>
-      <c r="CJ2" s="1" t="b">
+        <v>999</v>
+      </c>
+      <c r="CJ2" s="1">
+        <v>1</v>
+      </c>
+      <c r="CK2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="CL2" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="CM2" s="1">
+        <v>2</v>
+      </c>
+      <c r="CN2" s="1">
+        <v>10</v>
+      </c>
+      <c r="CO2" s="1">
+        <v>1</v>
+      </c>
+      <c r="CP2" s="1" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Working on splash attack functionality
</commit_message>
<xml_diff>
--- a/ProjectApopalypse_Unity/Excel/Units.xlsx
+++ b/ProjectApopalypse_Unity/Excel/Units.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectApopalypse\ProjectApopalypse_Unity\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC96B6AE-19BB-4E28-BF01-7E844E746FF4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80611D33-9781-4044-9E5B-555F22CBE638}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{3A2312A1-F630-46F4-AF7A-37D6220B2126}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
   <si>
     <t>technicalName</t>
   </si>
@@ -309,9 +309,6 @@
     <t>splashType</t>
   </si>
   <si>
-    <t>attackOrigin</t>
-  </si>
-  <si>
     <t>Targets</t>
   </si>
   <si>
@@ -331,6 +328,15 @@
   </si>
   <si>
     <t>salvoRate</t>
+  </si>
+  <si>
+    <t>targetAllies</t>
+  </si>
+  <si>
+    <t>targetEnemies</t>
+  </si>
+  <si>
+    <t>splashOrigin</t>
   </si>
 </sst>
 </file>
@@ -690,23 +696,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66FF625-BC64-4C5F-8916-6942D597EF48}">
-  <dimension ref="A1:CP2"/>
+  <dimension ref="A1:CR2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BS1" workbookViewId="0">
-      <selection activeCell="CL2" sqref="CL2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="7.8" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8.33203125" style="1" customWidth="1"/>
-    <col min="2" max="13" width="8.77734375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" style="1" customWidth="1"/>
-    <col min="15" max="88" width="8.88671875" style="1"/>
-    <col min="89" max="90" width="9.21875" style="1" customWidth="1"/>
-    <col min="91" max="16384" width="8.88671875" style="1"/>
+    <col min="2" max="15" width="8.77734375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="8.88671875" style="1" customWidth="1"/>
+    <col min="17" max="90" width="8.88671875" style="1"/>
+    <col min="91" max="92" width="9.21875" style="1" customWidth="1"/>
+    <col min="93" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:94" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -729,268 +735,274 @@
         <v>88</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AX1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="BA1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BT1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="BS1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="BT1" s="1" t="s">
+      <c r="BV1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="BU1" s="1" t="s">
+      <c r="BW1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="BV1" s="1" t="s">
+      <c r="BX1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="BW1" s="1" t="s">
+      <c r="BY1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="BX1" s="1" t="s">
+      <c r="BZ1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="BY1" s="1" t="s">
+      <c r="CA1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="BZ1" s="1" t="s">
+      <c r="CB1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="CA1" s="1" t="s">
+      <c r="CC1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="CB1" s="1" t="s">
+      <c r="CD1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="CC1" s="1" t="s">
+      <c r="CE1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="CD1" s="1" t="s">
+      <c r="CF1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="CE1" s="1" t="s">
+      <c r="CG1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="CF1" s="1" t="s">
+      <c r="CH1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="CG1" s="1" t="s">
+      <c r="CI1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="CH1" s="1" t="s">
+      <c r="CJ1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="CI1" s="1" t="s">
+      <c r="CK1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="CJ1" s="1" t="s">
+      <c r="CL1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="CK1" s="1" t="s">
+      <c r="CM1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="CL1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="CM1" s="1" t="s">
+      <c r="CN1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="CO1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="CP1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="CN1" s="1" t="s">
+      <c r="CQ1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="CO1" s="1" t="s">
+      <c r="CR1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="CP1" s="1" t="s">
-        <v>100</v>
-      </c>
     </row>
-    <row r="2" spans="1:94" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -1012,256 +1024,262 @@
       <c r="G2" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="N2" s="1">
-        <v>10</v>
-      </c>
-      <c r="O2" s="1">
-        <v>999</v>
-      </c>
       <c r="P2" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="1" t="b">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>999</v>
       </c>
       <c r="R2" s="1">
-        <v>10</v>
-      </c>
-      <c r="S2" s="1">
-        <v>999</v>
+        <v>1</v>
+      </c>
+      <c r="S2" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="T2" s="1">
-        <v>1</v>
-      </c>
-      <c r="U2" s="1" t="b">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="U2" s="1">
+        <v>999</v>
       </c>
       <c r="V2" s="1">
-        <v>10</v>
-      </c>
-      <c r="W2" s="1">
-        <v>999</v>
+        <v>1</v>
+      </c>
+      <c r="W2" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="X2" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y2" s="1" t="b">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>999</v>
       </c>
       <c r="Z2" s="1">
-        <v>10</v>
-      </c>
-      <c r="AA2" s="1">
-        <v>999</v>
+        <v>1</v>
+      </c>
+      <c r="AA2" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="AB2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AC2" s="1" t="b">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>999</v>
       </c>
       <c r="AD2" s="1">
-        <v>10</v>
-      </c>
-      <c r="AE2" s="1">
-        <v>999</v>
+        <v>1</v>
+      </c>
+      <c r="AE2" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="AF2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AG2" s="1" t="b">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>999</v>
       </c>
       <c r="AH2" s="1">
-        <v>10</v>
-      </c>
-      <c r="AI2" s="1">
-        <v>999</v>
+        <v>1</v>
+      </c>
+      <c r="AI2" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="AJ2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AK2" s="1" t="b">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="AK2" s="1">
+        <v>999</v>
       </c>
       <c r="AL2" s="1">
-        <v>10</v>
-      </c>
-      <c r="AM2" s="1">
-        <v>999</v>
+        <v>1</v>
+      </c>
+      <c r="AM2" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="AN2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AO2" s="1" t="b">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="AO2" s="1">
+        <v>999</v>
       </c>
       <c r="AP2" s="1">
-        <v>10</v>
-      </c>
-      <c r="AQ2" s="1">
-        <v>999</v>
+        <v>1</v>
+      </c>
+      <c r="AQ2" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="AR2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AS2" s="1" t="b">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="AS2" s="1">
+        <v>999</v>
       </c>
       <c r="AT2" s="1">
-        <v>10</v>
-      </c>
-      <c r="AU2" s="1">
-        <v>999</v>
+        <v>1</v>
+      </c>
+      <c r="AU2" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="AV2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AW2" s="1" t="b">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="AW2" s="1">
+        <v>999</v>
       </c>
       <c r="AX2" s="1">
-        <v>10</v>
-      </c>
-      <c r="AY2" s="1">
-        <v>999</v>
+        <v>1</v>
+      </c>
+      <c r="AY2" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="AZ2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BA2" s="1" t="b">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="BA2" s="1">
+        <v>999</v>
       </c>
       <c r="BB2" s="1">
-        <v>10</v>
-      </c>
-      <c r="BC2" s="1">
-        <v>999</v>
+        <v>1</v>
+      </c>
+      <c r="BC2" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="BD2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BE2" s="1" t="b">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="BE2" s="1">
+        <v>999</v>
       </c>
       <c r="BF2" s="1">
-        <v>10</v>
-      </c>
-      <c r="BG2" s="1">
-        <v>999</v>
+        <v>1</v>
+      </c>
+      <c r="BG2" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="BH2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BI2" s="1" t="b">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="BI2" s="1">
+        <v>999</v>
       </c>
       <c r="BJ2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BK2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BL2" s="1">
+        <v>3</v>
+      </c>
+      <c r="BM2" s="1">
+        <v>999</v>
+      </c>
+      <c r="BN2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BO2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BP2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BQ2" s="1">
+        <v>999</v>
+      </c>
+      <c r="BR2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BS2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BT2" s="1">
+        <v>10</v>
+      </c>
+      <c r="BU2" s="1">
+        <v>999</v>
+      </c>
+      <c r="BV2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BW2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BX2" s="1">
+        <v>10</v>
+      </c>
+      <c r="BY2" s="1">
+        <v>999</v>
+      </c>
+      <c r="BZ2" s="1">
+        <v>1</v>
+      </c>
+      <c r="CA2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="CB2" s="1">
+        <v>10</v>
+      </c>
+      <c r="CC2" s="1">
+        <v>999</v>
+      </c>
+      <c r="CD2" s="1">
+        <v>1</v>
+      </c>
+      <c r="CE2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="CF2" s="1">
+        <v>10</v>
+      </c>
+      <c r="CG2" s="1">
+        <v>999</v>
+      </c>
+      <c r="CH2" s="1">
+        <v>1</v>
+      </c>
+      <c r="CI2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="CJ2" s="1">
+        <v>10</v>
+      </c>
+      <c r="CK2" s="1">
+        <v>999</v>
+      </c>
+      <c r="CL2" s="1">
+        <v>1</v>
+      </c>
+      <c r="CM2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="CN2" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="CO2" s="1">
         <v>2</v>
       </c>
-      <c r="BK2" s="1">
-        <v>999</v>
-      </c>
-      <c r="BL2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BM2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="BN2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BO2" s="1">
-        <v>999</v>
-      </c>
-      <c r="BP2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BQ2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="BR2" s="1">
-        <v>10</v>
-      </c>
-      <c r="BS2" s="1">
-        <v>999</v>
-      </c>
-      <c r="BT2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BU2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="BV2" s="1">
-        <v>10</v>
-      </c>
-      <c r="BW2" s="1">
-        <v>999</v>
-      </c>
-      <c r="BX2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BY2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="BZ2" s="1">
-        <v>10</v>
-      </c>
-      <c r="CA2" s="1">
-        <v>999</v>
-      </c>
-      <c r="CB2" s="1">
-        <v>1</v>
-      </c>
-      <c r="CC2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="CD2" s="1">
-        <v>10</v>
-      </c>
-      <c r="CE2" s="1">
-        <v>999</v>
-      </c>
-      <c r="CF2" s="1">
-        <v>1</v>
-      </c>
-      <c r="CG2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="CH2" s="1">
-        <v>10</v>
-      </c>
-      <c r="CI2" s="1">
-        <v>999</v>
-      </c>
-      <c r="CJ2" s="1">
-        <v>1</v>
-      </c>
-      <c r="CK2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="CL2" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="CM2" s="1">
-        <v>2</v>
-      </c>
-      <c r="CN2" s="1">
-        <v>10</v>
-      </c>
-      <c r="CO2" s="1">
-        <v>1</v>
-      </c>
-      <c r="CP2" s="1" t="b">
+      <c r="CP2" s="1">
+        <v>10</v>
+      </c>
+      <c r="CQ2" s="1">
+        <v>1</v>
+      </c>
+      <c r="CR2" s="1" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More splash work, lines
</commit_message>
<xml_diff>
--- a/ProjectApopalypse_Unity/Excel/Units.xlsx
+++ b/ProjectApopalypse_Unity/Excel/Units.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectApopalypse\ProjectApopalypse_Unity\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80611D33-9781-4044-9E5B-555F22CBE638}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACF1E75-AB83-429D-9173-044948A0C193}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{3A2312A1-F630-46F4-AF7A-37D6220B2126}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="109">
   <si>
     <t>technicalName</t>
   </si>
@@ -81,15 +81,9 @@
     <t>actMoveSpeed</t>
   </si>
   <si>
-    <t>defaultUnit</t>
-  </si>
-  <si>
     <t>displayName</t>
   </si>
   <si>
-    <t>Default Unit</t>
-  </si>
-  <si>
     <t>actHealthMax</t>
   </si>
   <si>
@@ -312,9 +306,6 @@
     <t>Targets</t>
   </si>
   <si>
-    <t>Sphere</t>
-  </si>
-  <si>
     <t>actTargets</t>
   </si>
   <si>
@@ -337,6 +328,30 @@
   </si>
   <si>
     <t>splashOrigin</t>
+  </si>
+  <si>
+    <t>Line</t>
+  </si>
+  <si>
+    <t>defaultSplashUnit</t>
+  </si>
+  <si>
+    <t>Default Splash Unit</t>
+  </si>
+  <si>
+    <t>defaultDirectUnit</t>
+  </si>
+  <si>
+    <t>Default Direct Unit</t>
+  </si>
+  <si>
+    <t>Ground</t>
+  </si>
+  <si>
+    <t>Self</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -386,7 +401,1772 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="98">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -397,6 +2177,111 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C2383A53-3A2F-40EF-B721-6DA1839BF909}" name="Table1" displayName="Table1" ref="A1:CR3" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96">
+  <autoFilter ref="A1:CR3" xr:uid="{9EC39B5B-8F44-472E-918B-DBA77F12954E}"/>
+  <tableColumns count="96">
+    <tableColumn id="1" xr3:uid="{89B66E7D-F1B0-4F11-A8C4-437D2EE54D17}" name="technicalName" dataDxfId="95"/>
+    <tableColumn id="2" xr3:uid="{CC988DFD-F98F-486F-AD81-B53A776A7D5A}" name="displayName" dataDxfId="94"/>
+    <tableColumn id="3" xr3:uid="{44D15C63-6D62-495D-85F5-9CCF58B79FDE}" name="description" dataDxfId="93"/>
+    <tableColumn id="4" xr3:uid="{545FCCFA-9A67-4E7B-9071-9F021AE4B2AD}" name="rank" dataDxfId="92"/>
+    <tableColumn id="5" xr3:uid="{28D65B36-0E27-4A75-8220-E8BC8D82D324}" name="canMove" dataDxfId="91"/>
+    <tableColumn id="6" xr3:uid="{A42853E4-5F24-497D-870A-62AEF57FFEED}" name="canAttack" dataDxfId="90"/>
+    <tableColumn id="7" xr3:uid="{D2449210-25FD-4C20-88AB-9E6581657C27}" name="moveType" dataDxfId="89"/>
+    <tableColumn id="8" xr3:uid="{092C91A1-3DB7-4450-8F05-AAD1CDA0F14C}" name="targetAllies" dataDxfId="88"/>
+    <tableColumn id="9" xr3:uid="{8CE7E365-3646-4682-B988-BCD9972D5CE3}" name="targetEnemies" dataDxfId="87"/>
+    <tableColumn id="10" xr3:uid="{49914703-F632-4F6B-A5D7-AF9C3521999F}" name="splashOrigin" dataDxfId="86"/>
+    <tableColumn id="11" xr3:uid="{9CCCDE5D-9BBE-4F02-9B68-128D58CC29FE}" name="splashType" dataDxfId="85"/>
+    <tableColumn id="12" xr3:uid="{A4D3FB9F-46F6-42E3-A00E-F3D2F6D4DB38}" name="passive1" dataDxfId="84"/>
+    <tableColumn id="13" xr3:uid="{8385E9D4-FD43-4930-B457-432C24E6790C}" name="passive2" dataDxfId="83"/>
+    <tableColumn id="14" xr3:uid="{1D9163BD-EEA7-4F85-9C91-2860370D68BC}" name="passive3" dataDxfId="82"/>
+    <tableColumn id="15" xr3:uid="{5B82B078-1E92-472B-8518-6058FC12E019}" name="passive4" dataDxfId="81"/>
+    <tableColumn id="16" xr3:uid="{C23B8D87-2A5D-43F6-90EA-5864E31B464F}" name="actHealth" dataDxfId="80"/>
+    <tableColumn id="17" xr3:uid="{43710A8A-04CB-4095-A2EA-1A4836E1C6FB}" name="actHealthMax" dataDxfId="79"/>
+    <tableColumn id="18" xr3:uid="{F86967A0-EBB2-44BA-8F01-45A812785C4C}" name="actHealthMin" dataDxfId="78"/>
+    <tableColumn id="19" xr3:uid="{CC5D0B14-3999-4739-9D1E-E70BE1C42C8F}" name="actHealthLocked" dataDxfId="77"/>
+    <tableColumn id="20" xr3:uid="{15A9D1C6-243B-44BD-99F7-A4E5FA623969}" name="actBaseArmor" dataDxfId="76"/>
+    <tableColumn id="21" xr3:uid="{8BC5E85F-33EB-4E7B-86B8-0ECC89EACE93}" name="actBaseArmorMax" dataDxfId="75"/>
+    <tableColumn id="22" xr3:uid="{7ABC5504-21B0-4D00-B6B3-288BC5483B9D}" name="actBaseArmorMin" dataDxfId="74"/>
+    <tableColumn id="23" xr3:uid="{57692A96-1B3E-483C-A7DA-DC8CE67C6151}" name="actBaseArmorLocked" dataDxfId="73"/>
+    <tableColumn id="24" xr3:uid="{362B58B0-6FE6-4632-A1A5-C6F380A9C25D}" name="actTroopArmor" dataDxfId="72"/>
+    <tableColumn id="25" xr3:uid="{FBD59B2C-0A7F-4C4F-8ACA-D3F01279358E}" name="actTroopArmorMax" dataDxfId="71"/>
+    <tableColumn id="26" xr3:uid="{45246D11-B2D4-440F-96CD-66DAD24F6398}" name="actTroopArmorMin" dataDxfId="70"/>
+    <tableColumn id="27" xr3:uid="{CF362526-F313-45DB-BC95-A8A7C13FFA44}" name="actTroopArmorLocked" dataDxfId="69"/>
+    <tableColumn id="28" xr3:uid="{3A2B1E3E-DF2F-4CFE-99EE-FDDCA94C9DAC}" name="actStructureArmor" dataDxfId="68"/>
+    <tableColumn id="29" xr3:uid="{D18FD356-5FD0-4B4A-B060-4CE21A3512F0}" name="actStructureArmorMax" dataDxfId="67"/>
+    <tableColumn id="30" xr3:uid="{83839766-ECDF-4704-B2F6-F192D47A488C}" name="actStructureArmorMin" dataDxfId="66"/>
+    <tableColumn id="31" xr3:uid="{6DA3CD16-3527-4CB8-BF08-81CCD3793991}" name="actStructureArmorLocked" dataDxfId="65"/>
+    <tableColumn id="32" xr3:uid="{2F0AC323-43E2-4846-A4B1-4A1B5C25DD4D}" name="actDirectArmor" dataDxfId="64"/>
+    <tableColumn id="33" xr3:uid="{270FCC45-AF5F-454E-B48A-4BAC176F4A3F}" name="actDirectArmorMax" dataDxfId="63"/>
+    <tableColumn id="34" xr3:uid="{3329CEA9-8AEA-4E45-939D-634B8BEFEA38}" name="actDirectArmorMin" dataDxfId="62"/>
+    <tableColumn id="35" xr3:uid="{86E02453-A982-46A2-A0BF-43112926B026}" name="actDirectArmorLocked" dataDxfId="61"/>
+    <tableColumn id="36" xr3:uid="{D86A8383-F81D-42CF-B3CC-31CD28A63610}" name="actSplashArmor" dataDxfId="60"/>
+    <tableColumn id="37" xr3:uid="{23680859-40C1-41CD-ABE3-B8703F9B2F5B}" name="actSplashArmorMax" dataDxfId="59"/>
+    <tableColumn id="38" xr3:uid="{02A40395-83DE-4FE4-9C59-226938800BF1}" name="actSplashArmorMin" dataDxfId="58"/>
+    <tableColumn id="39" xr3:uid="{320B4EF6-69B4-47C0-A80A-599304A41B4A}" name="actSplashArmorLocked" dataDxfId="57"/>
+    <tableColumn id="40" xr3:uid="{B795FB0F-BE6F-463A-BF4C-6915B32E5B56}" name="actBaseDamage" dataDxfId="56"/>
+    <tableColumn id="41" xr3:uid="{CE98D0C8-8C9F-4DAD-AA2A-CD32E574E363}" name="actBaseDamageMax" dataDxfId="55"/>
+    <tableColumn id="42" xr3:uid="{A284F53E-3A21-41EF-A654-440E2816DD9E}" name="actBaseDamageMin" dataDxfId="54"/>
+    <tableColumn id="43" xr3:uid="{8AC1F35A-0E3B-49C3-9F2A-39A82607F396}" name="actBaseDamageLocked" dataDxfId="53"/>
+    <tableColumn id="44" xr3:uid="{1D185D06-BB88-4702-9096-A7F0244A4B80}" name="actTroopDamage" dataDxfId="52"/>
+    <tableColumn id="45" xr3:uid="{EBED8B3A-0C27-4991-AA22-53E412F08CA4}" name="actTroopDamageMax" dataDxfId="51"/>
+    <tableColumn id="46" xr3:uid="{B0559B8A-AAD6-42EA-839E-36496B615CCF}" name="actTroopDamageMin" dataDxfId="50"/>
+    <tableColumn id="47" xr3:uid="{C90063C2-B909-4303-A1A7-C0BEDC53791F}" name="actTroopDamageLocked" dataDxfId="49"/>
+    <tableColumn id="48" xr3:uid="{4C0116C3-0E2F-492F-9470-74D1580385B4}" name="actCoreDamage" dataDxfId="48"/>
+    <tableColumn id="49" xr3:uid="{24F8C556-C9B1-4C1A-A1BD-6DAD33E448CE}" name="actCoreDamageMax" dataDxfId="47"/>
+    <tableColumn id="50" xr3:uid="{8CC41FF1-A232-4542-AE1E-9C5011F3DC67}" name="actCoreDamageMin" dataDxfId="46"/>
+    <tableColumn id="51" xr3:uid="{2E41712B-CD28-4824-B982-D8C63C9DDF3B}" name="actCoreDamageLocked" dataDxfId="45"/>
+    <tableColumn id="52" xr3:uid="{5945AECC-BE9B-482B-89DA-165345C08DF0}" name="actChestDamage" dataDxfId="44"/>
+    <tableColumn id="53" xr3:uid="{3182A3BD-B750-47DE-A267-519174025FCB}" name="actChestDamageMax" dataDxfId="43"/>
+    <tableColumn id="54" xr3:uid="{165EECF5-96C4-46AA-928C-C64728D77043}" name="actChestDamageMin" dataDxfId="42"/>
+    <tableColumn id="55" xr3:uid="{86A03080-0190-4A6C-8988-742D11593A82}" name="actChestDamageLocked" dataDxfId="41"/>
+    <tableColumn id="56" xr3:uid="{E4F5E069-D5B8-4C4A-84BD-5111B1EA1084}" name="actDirectDamage" dataDxfId="40"/>
+    <tableColumn id="57" xr3:uid="{1DC47B3C-B438-4CA2-A801-003138AAFC4E}" name="actDirectDamageMax" dataDxfId="39"/>
+    <tableColumn id="58" xr3:uid="{C1DF00D9-E15D-46FB-BCFF-81305B014ACB}" name="actDirectDamageMin" dataDxfId="38"/>
+    <tableColumn id="59" xr3:uid="{66DDCBB2-CD84-484B-B7DD-B09744CB9376}" name="actDirectDamageLocked" dataDxfId="37"/>
+    <tableColumn id="60" xr3:uid="{86673E61-F62F-49A4-B32F-A0C1676E7BAA}" name="actSplashDamage" dataDxfId="36"/>
+    <tableColumn id="61" xr3:uid="{9AB4867E-6AC7-458C-892E-82641A383927}" name="actSplashDamageMax" dataDxfId="35"/>
+    <tableColumn id="62" xr3:uid="{45E931B0-CA14-4F33-A2DB-9125F624DB04}" name="actSplashDamageMin" dataDxfId="34"/>
+    <tableColumn id="63" xr3:uid="{30016B0F-7DD6-4F4A-90C7-BE910DF78352}" name="actSplashDamageLocked" dataDxfId="33"/>
+    <tableColumn id="64" xr3:uid="{62F58218-5D7D-4DA9-AE0D-851EDEF55C80}" name="actCooldown" dataDxfId="32"/>
+    <tableColumn id="65" xr3:uid="{E1A7B3A0-3825-4138-84E0-C4F504E7591F}" name="actCooldownMax" dataDxfId="31"/>
+    <tableColumn id="66" xr3:uid="{BB2E512D-C314-4C4B-BFC0-1036086B5CD6}" name="actCooldownMin" dataDxfId="30"/>
+    <tableColumn id="67" xr3:uid="{1AF3441D-DEAE-4FC4-A41B-9D21B8A3A5EF}" name="actCooldownLocked" dataDxfId="29"/>
+    <tableColumn id="68" xr3:uid="{8ACCD9C2-2CF8-41EF-B81C-847DDD2BA350}" name="actChargeTime" dataDxfId="28"/>
+    <tableColumn id="69" xr3:uid="{411C34B1-AA06-4150-9DAB-58823AF07DB2}" name="actChargeTimeMax" dataDxfId="27"/>
+    <tableColumn id="70" xr3:uid="{DFC87401-3400-4D87-8BC0-5DCA6DB5A1F6}" name="actChargeTimeMin" dataDxfId="26"/>
+    <tableColumn id="71" xr3:uid="{0CDC35B3-44BB-40CC-82B1-18E03AA9B7A4}" name="actChargeTimeLocked" dataDxfId="25"/>
+    <tableColumn id="72" xr3:uid="{F5891BD0-6CE3-4542-B617-DA5DE07CA318}" name="actSplashRadius" dataDxfId="24"/>
+    <tableColumn id="73" xr3:uid="{57A71DFE-1CCD-4C76-BE80-D42995942AF6}" name="actSplashRadiusMax" dataDxfId="23"/>
+    <tableColumn id="74" xr3:uid="{60002B8B-A779-44D6-86B3-1239FE85C73C}" name="actSplashRadiusMin" dataDxfId="22"/>
+    <tableColumn id="75" xr3:uid="{07B62B07-DBEA-42CE-8050-4616D06262EC}" name="actSplashRadiusLocked" dataDxfId="21"/>
+    <tableColumn id="76" xr3:uid="{6D9CD8B6-0100-483C-BF80-4C09B351C28B}" name="actRange" dataDxfId="20"/>
+    <tableColumn id="77" xr3:uid="{4B373AB3-4D03-426A-827D-838E56115142}" name="actRangeMax" dataDxfId="19"/>
+    <tableColumn id="78" xr3:uid="{FD943F32-7F2B-4D0F-9EB8-3D9E6FDF5B0F}" name="actRangeMin" dataDxfId="18"/>
+    <tableColumn id="79" xr3:uid="{C4A527EB-C773-4A60-8864-562FF42FF82E}" name="actRangeLocked" dataDxfId="17"/>
+    <tableColumn id="80" xr3:uid="{71CDC41A-8B45-459F-A6F6-1B177A31D702}" name="actMoveSpeed" dataDxfId="16"/>
+    <tableColumn id="81" xr3:uid="{00E6FF2F-8B9D-4FFE-9845-B4E3312329C9}" name="actMoveSpeedMax" dataDxfId="15"/>
+    <tableColumn id="82" xr3:uid="{B20A486B-5C8A-4740-B342-3A4482DCBFD2}" name="actMoveSpeedMin" dataDxfId="14"/>
+    <tableColumn id="83" xr3:uid="{00F3DDF5-8176-40D7-B259-D2E87B983032}" name="actMoveSpeedLocked" dataDxfId="13"/>
+    <tableColumn id="84" xr3:uid="{FC414463-68F1-46BE-BDE9-FDD5B8BFDEE8}" name="actCharges" dataDxfId="12"/>
+    <tableColumn id="85" xr3:uid="{A0268830-0315-4432-B4F5-9202549B3096}" name="actChargesMax" dataDxfId="11"/>
+    <tableColumn id="86" xr3:uid="{53B2773A-4DDC-42C7-B66F-70DB32E12775}" name="actChargesMin" dataDxfId="10"/>
+    <tableColumn id="87" xr3:uid="{2B807DB6-B45A-42F6-91BA-A7C0CEA25910}" name="actChargesLocked" dataDxfId="9"/>
+    <tableColumn id="88" xr3:uid="{AA61D924-F131-4E94-A97F-AB3A1B1CB87B}" name="actSalvo" dataDxfId="8"/>
+    <tableColumn id="89" xr3:uid="{D14D9EE8-6C21-4E59-8D36-D5057474DFFD}" name="actSalvoMax" dataDxfId="7"/>
+    <tableColumn id="90" xr3:uid="{C66167A7-DE1C-4383-A438-6C03EFB8B53E}" name="actSalvoMin" dataDxfId="6"/>
+    <tableColumn id="91" xr3:uid="{E399206F-2BE7-453B-8491-DCD1BB3BDEB2}" name="actSalvoLocked" dataDxfId="5"/>
+    <tableColumn id="92" xr3:uid="{D220613B-CCAF-4C49-88A2-1A032E016F37}" name="salvoRate" dataDxfId="4"/>
+    <tableColumn id="93" xr3:uid="{BA2E889E-86F5-4ECC-B58A-1582BAC8E743}" name="actTargets" dataDxfId="3"/>
+    <tableColumn id="94" xr3:uid="{10565265-0646-414F-A9E2-038BDADDF5DF}" name="actTargetsMax" dataDxfId="2"/>
+    <tableColumn id="95" xr3:uid="{22FF9324-3AA4-448A-A7BB-F0967257A25E}" name="actTargetsMin" dataDxfId="1"/>
+    <tableColumn id="96" xr3:uid="{2EB715CC-324F-4120-8079-DF73170EF911}" name="actTargetsLocked" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -696,20 +2581,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66FF625-BC64-4C5F-8916-6942D597EF48}">
-  <dimension ref="A1:CR2"/>
+  <dimension ref="A1:CR3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="CR3" sqref="CR3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="7.8" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" style="1" customWidth="1"/>
-    <col min="2" max="15" width="8.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="1" customWidth="1"/>
+    <col min="3" max="8" width="8.77734375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.21875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.21875" style="1" customWidth="1"/>
+    <col min="11" max="15" width="8.77734375" style="1" customWidth="1"/>
     <col min="16" max="16" width="8.88671875" style="1" customWidth="1"/>
-    <col min="17" max="90" width="8.88671875" style="1"/>
-    <col min="91" max="92" width="9.21875" style="1" customWidth="1"/>
-    <col min="93" max="16384" width="8.88671875" style="1"/>
+    <col min="17" max="17" width="10" style="1" customWidth="1"/>
+    <col min="18" max="18" width="9.6640625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="11.77734375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="10.21875" style="1" customWidth="1"/>
+    <col min="21" max="21" width="12.33203125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="12" style="1" customWidth="1"/>
+    <col min="23" max="23" width="14.109375" style="1" customWidth="1"/>
+    <col min="24" max="24" width="10.5546875" style="1" customWidth="1"/>
+    <col min="25" max="25" width="12.6640625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="12.33203125" style="1" customWidth="1"/>
+    <col min="27" max="27" width="14.44140625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="12.33203125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="14.44140625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="14.109375" style="1" customWidth="1"/>
+    <col min="31" max="31" width="16.21875" style="1" customWidth="1"/>
+    <col min="32" max="32" width="10.5546875" style="1" customWidth="1"/>
+    <col min="33" max="33" width="12.6640625" style="1" customWidth="1"/>
+    <col min="34" max="34" width="12.33203125" style="1" customWidth="1"/>
+    <col min="35" max="35" width="14.44140625" style="1" customWidth="1"/>
+    <col min="36" max="36" width="11.109375" style="1" customWidth="1"/>
+    <col min="37" max="37" width="13.21875" style="1" customWidth="1"/>
+    <col min="38" max="38" width="12.88671875" style="1" customWidth="1"/>
+    <col min="39" max="39" width="15" style="1" customWidth="1"/>
+    <col min="40" max="40" width="11.5546875" style="1" customWidth="1"/>
+    <col min="41" max="41" width="13.6640625" style="1" customWidth="1"/>
+    <col min="42" max="42" width="13.33203125" style="1" customWidth="1"/>
+    <col min="43" max="43" width="15.44140625" style="1" customWidth="1"/>
+    <col min="44" max="44" width="11.88671875" style="1" customWidth="1"/>
+    <col min="45" max="45" width="14" style="1" customWidth="1"/>
+    <col min="46" max="46" width="13.6640625" style="1" customWidth="1"/>
+    <col min="47" max="47" width="15.77734375" style="1" customWidth="1"/>
+    <col min="48" max="48" width="11.33203125" style="1" customWidth="1"/>
+    <col min="49" max="49" width="13.44140625" style="1" customWidth="1"/>
+    <col min="50" max="50" width="13.109375" style="1" customWidth="1"/>
+    <col min="51" max="51" width="15.21875" style="1" customWidth="1"/>
+    <col min="52" max="52" width="11.88671875" style="1" customWidth="1"/>
+    <col min="53" max="53" width="14" style="1" customWidth="1"/>
+    <col min="54" max="54" width="13.6640625" style="1" customWidth="1"/>
+    <col min="55" max="55" width="15.77734375" style="1" customWidth="1"/>
+    <col min="56" max="56" width="11.88671875" style="1" customWidth="1"/>
+    <col min="57" max="57" width="14" style="1" customWidth="1"/>
+    <col min="58" max="58" width="13.6640625" style="1" customWidth="1"/>
+    <col min="59" max="59" width="15.77734375" style="1" customWidth="1"/>
+    <col min="60" max="60" width="12.44140625" style="1" customWidth="1"/>
+    <col min="61" max="61" width="14.5546875" style="1" customWidth="1"/>
+    <col min="62" max="62" width="14.21875" style="1" customWidth="1"/>
+    <col min="63" max="63" width="16.33203125" style="1" customWidth="1"/>
+    <col min="64" max="64" width="9.6640625" style="1" customWidth="1"/>
+    <col min="65" max="65" width="11.77734375" style="1" customWidth="1"/>
+    <col min="66" max="66" width="11.44140625" style="1" customWidth="1"/>
+    <col min="67" max="67" width="13.5546875" style="1" customWidth="1"/>
+    <col min="68" max="68" width="10.77734375" style="1" customWidth="1"/>
+    <col min="69" max="69" width="12.88671875" style="1" customWidth="1"/>
+    <col min="70" max="70" width="12.5546875" style="1" customWidth="1"/>
+    <col min="71" max="71" width="14.6640625" style="1" customWidth="1"/>
+    <col min="72" max="72" width="11.6640625" style="1" customWidth="1"/>
+    <col min="73" max="73" width="13.77734375" style="1" customWidth="1"/>
+    <col min="74" max="74" width="13.44140625" style="1" customWidth="1"/>
+    <col min="75" max="75" width="15.5546875" style="1" customWidth="1"/>
+    <col min="76" max="76" width="8.88671875" style="1"/>
+    <col min="77" max="77" width="10.109375" style="1" customWidth="1"/>
+    <col min="78" max="78" width="9.77734375" style="1" customWidth="1"/>
+    <col min="79" max="79" width="11.88671875" style="1" customWidth="1"/>
+    <col min="80" max="80" width="10.77734375" style="1" customWidth="1"/>
+    <col min="81" max="81" width="12.88671875" style="1" customWidth="1"/>
+    <col min="82" max="82" width="12.5546875" style="1" customWidth="1"/>
+    <col min="83" max="83" width="14.6640625" style="1" customWidth="1"/>
+    <col min="84" max="84" width="8.88671875" style="1"/>
+    <col min="85" max="85" width="11" style="1" customWidth="1"/>
+    <col min="86" max="86" width="10.6640625" style="1" customWidth="1"/>
+    <col min="87" max="87" width="12.77734375" style="1" customWidth="1"/>
+    <col min="88" max="88" width="8.88671875" style="1"/>
+    <col min="89" max="89" width="9.5546875" style="1" customWidth="1"/>
+    <col min="90" max="90" width="9.21875" style="1" customWidth="1"/>
+    <col min="91" max="91" width="11.33203125" style="1" customWidth="1"/>
+    <col min="92" max="92" width="9.21875" style="1" customWidth="1"/>
+    <col min="93" max="93" width="8.88671875" style="1"/>
+    <col min="94" max="94" width="10.5546875" style="1" customWidth="1"/>
+    <col min="95" max="95" width="10.21875" style="1" customWidth="1"/>
+    <col min="96" max="96" width="12.33203125" style="1" customWidth="1"/>
+    <col min="97" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.15">
@@ -717,303 +2684,303 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="U1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="Y1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="AF1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="AG1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI1" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="AJ1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="AK1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AM1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="AN1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="AO1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="AR1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="AS1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AU1" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="AV1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="AW1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AY1" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="AZ1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="BA1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="BC1" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="BB1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="BD1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="BE1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BG1" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="BF1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="BG1" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="BH1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="BI1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BK1" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="BJ1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="BK1" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="BL1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="BM1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BO1" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="BN1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="BO1" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="BP1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="BQ1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BS1" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="BR1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="BS1" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="BT1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="BU1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BW1" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="BV1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="BW1" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="BX1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="BY1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BZ1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="CA1" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="BZ1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="CA1" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="CB1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="CC1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="CD1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="CE1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="CD1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="CE1" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="CF1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="CG1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="CH1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="CG1" s="1" t="s">
+      <c r="CI1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="CH1" s="1" t="s">
+      <c r="CJ1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="CI1" s="1" t="s">
+      <c r="CK1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="CJ1" s="1" t="s">
+      <c r="CL1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="CK1" s="1" t="s">
+      <c r="CM1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="CL1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="CM1" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="CN1" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="CO1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="CP1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="CQ1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="CR1" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="CP1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="CQ1" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="CR1" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>102</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>103</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E2" s="1" t="b">
         <v>1</v>
@@ -1022,7 +2989,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H2" s="1" t="b">
         <v>0</v>
@@ -1031,16 +2998,16 @@
         <v>1</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="P2" s="1">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="Q2" s="1">
         <v>999</v>
@@ -1052,7 +3019,7 @@
         <v>0</v>
       </c>
       <c r="T2" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="U2" s="1">
         <v>999</v>
@@ -1064,7 +3031,7 @@
         <v>0</v>
       </c>
       <c r="X2" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="Y2" s="1">
         <v>999</v>
@@ -1076,7 +3043,7 @@
         <v>0</v>
       </c>
       <c r="AB2" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AC2" s="1">
         <v>999</v>
@@ -1088,7 +3055,7 @@
         <v>0</v>
       </c>
       <c r="AF2" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AG2" s="1">
         <v>999</v>
@@ -1100,7 +3067,7 @@
         <v>0</v>
       </c>
       <c r="AJ2" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AK2" s="1">
         <v>999</v>
@@ -1112,7 +3079,7 @@
         <v>0</v>
       </c>
       <c r="AN2" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="AO2" s="1">
         <v>999</v>
@@ -1124,7 +3091,7 @@
         <v>0</v>
       </c>
       <c r="AR2" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AS2" s="1">
         <v>999</v>
@@ -1136,7 +3103,7 @@
         <v>0</v>
       </c>
       <c r="AV2" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AW2" s="1">
         <v>999</v>
@@ -1148,7 +3115,7 @@
         <v>0</v>
       </c>
       <c r="AZ2" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="BA2" s="1">
         <v>999</v>
@@ -1160,7 +3127,7 @@
         <v>0</v>
       </c>
       <c r="BD2" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="BE2" s="1">
         <v>999</v>
@@ -1172,7 +3139,7 @@
         <v>0</v>
       </c>
       <c r="BH2" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="BI2" s="1">
         <v>999</v>
@@ -1184,31 +3151,31 @@
         <v>0</v>
       </c>
       <c r="BL2" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BM2" s="1">
         <v>999</v>
       </c>
       <c r="BN2" s="1">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="BO2" s="1" t="b">
         <v>0</v>
       </c>
       <c r="BP2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ2" s="1">
         <v>999</v>
       </c>
       <c r="BR2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS2" s="1" t="b">
         <v>0</v>
       </c>
       <c r="BT2" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="BU2" s="1">
         <v>999</v>
@@ -1220,7 +3187,7 @@
         <v>0</v>
       </c>
       <c r="BX2" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="BY2" s="1">
         <v>999</v>
@@ -1232,7 +3199,7 @@
         <v>0</v>
       </c>
       <c r="CB2" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="CC2" s="1">
         <v>999</v>
@@ -1244,7 +3211,7 @@
         <v>0</v>
       </c>
       <c r="CF2" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="CG2" s="1">
         <v>999</v>
@@ -1256,7 +3223,7 @@
         <v>0</v>
       </c>
       <c r="CJ2" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="CK2" s="1">
         <v>999</v>
@@ -1271,7 +3238,7 @@
         <v>0.1</v>
       </c>
       <c r="CO2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="CP2" s="1">
         <v>10</v>
@@ -1280,11 +3247,295 @@
         <v>1</v>
       </c>
       <c r="CR2" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:96" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="P3" s="1">
+        <v>50</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>999</v>
+      </c>
+      <c r="R3" s="1">
+        <v>1</v>
+      </c>
+      <c r="S3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="T3" s="1">
+        <v>0</v>
+      </c>
+      <c r="U3" s="1">
+        <v>999</v>
+      </c>
+      <c r="V3" s="1">
+        <v>1</v>
+      </c>
+      <c r="W3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="X3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>999</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>999</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="1">
+        <v>999</v>
+      </c>
+      <c r="AH3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="1">
+        <v>999</v>
+      </c>
+      <c r="AL3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AM3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AO3" s="1">
+        <v>999</v>
+      </c>
+      <c r="AP3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS3" s="1">
+        <v>999</v>
+      </c>
+      <c r="AT3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW3" s="1">
+        <v>999</v>
+      </c>
+      <c r="AX3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AZ3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA3" s="1">
+        <v>999</v>
+      </c>
+      <c r="BB3" s="1">
+        <v>1</v>
+      </c>
+      <c r="BC3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BD3" s="1">
+        <v>1</v>
+      </c>
+      <c r="BE3" s="1">
+        <v>999</v>
+      </c>
+      <c r="BF3" s="1">
+        <v>1</v>
+      </c>
+      <c r="BG3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BH3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI3" s="1">
+        <v>999</v>
+      </c>
+      <c r="BJ3" s="1">
+        <v>1</v>
+      </c>
+      <c r="BK3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BL3" s="1">
+        <v>2</v>
+      </c>
+      <c r="BM3" s="1">
+        <v>999</v>
+      </c>
+      <c r="BN3" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="BO3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BP3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BQ3" s="1">
+        <v>999</v>
+      </c>
+      <c r="BR3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BS3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BT3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BU3" s="1">
+        <v>999</v>
+      </c>
+      <c r="BV3" s="1">
+        <v>1</v>
+      </c>
+      <c r="BW3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BX3" s="1">
+        <v>2</v>
+      </c>
+      <c r="BY3" s="1">
+        <v>999</v>
+      </c>
+      <c r="BZ3" s="1">
+        <v>1</v>
+      </c>
+      <c r="CA3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="CB3" s="1">
+        <v>5</v>
+      </c>
+      <c r="CC3" s="1">
+        <v>999</v>
+      </c>
+      <c r="CD3" s="1">
+        <v>1</v>
+      </c>
+      <c r="CE3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="CF3" s="1">
+        <v>1</v>
+      </c>
+      <c r="CG3" s="1">
+        <v>999</v>
+      </c>
+      <c r="CH3" s="1">
+        <v>1</v>
+      </c>
+      <c r="CI3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="CJ3" s="1">
+        <v>0</v>
+      </c>
+      <c r="CK3" s="1">
+        <v>999</v>
+      </c>
+      <c r="CL3" s="1">
+        <v>1</v>
+      </c>
+      <c r="CM3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="CN3" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="CO3" s="1">
+        <v>1</v>
+      </c>
+      <c r="CP3" s="1">
+        <v>10</v>
+      </c>
+      <c r="CQ3" s="1">
+        <v>1</v>
+      </c>
+      <c r="CR3" s="1" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added a temp project to my project to grab some free scripts woot woot
</commit_message>
<xml_diff>
--- a/ProjectApopalypse_Unity/Excel/Units.xlsx
+++ b/ProjectApopalypse_Unity/Excel/Units.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectApopalypse\ProjectApopalypse_Unity\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACF1E75-AB83-429D-9173-044948A0C193}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22583F06-5F32-48FC-A5BB-50DB360C22C9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{3A2312A1-F630-46F4-AF7A-37D6220B2126}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="112">
   <si>
     <t>technicalName</t>
   </si>
@@ -352,6 +352,15 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>ehtan</t>
+  </si>
+  <si>
+    <t>EHTAN</t>
+  </si>
+  <si>
+    <t>iithishasjief Njeofjo</t>
   </si>
 </sst>
 </file>
@@ -2180,8 +2189,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C2383A53-3A2F-40EF-B721-6DA1839BF909}" name="Table1" displayName="Table1" ref="A1:CR3" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96">
-  <autoFilter ref="A1:CR3" xr:uid="{9EC39B5B-8F44-472E-918B-DBA77F12954E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C2383A53-3A2F-40EF-B721-6DA1839BF909}" name="Table1" displayName="Table1" ref="A1:CR4" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96">
+  <autoFilter ref="A1:CR4" xr:uid="{9EC39B5B-8F44-472E-918B-DBA77F12954E}"/>
   <tableColumns count="96">
     <tableColumn id="1" xr3:uid="{89B66E7D-F1B0-4F11-A8C4-437D2EE54D17}" name="technicalName" dataDxfId="95"/>
     <tableColumn id="2" xr3:uid="{CC988DFD-F98F-486F-AD81-B53A776A7D5A}" name="displayName" dataDxfId="94"/>
@@ -2581,10 +2590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66FF625-BC64-4C5F-8916-6942D597EF48}">
-  <dimension ref="A1:CR3"/>
+  <dimension ref="A1:CR4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="CR3" sqref="CR3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="7.8" x14ac:dyDescent="0.15"/>
@@ -3531,6 +3540,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:96" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Passive abilities work #1
</commit_message>
<xml_diff>
--- a/ProjectApopalypse_Unity/Excel/Units.xlsx
+++ b/ProjectApopalypse_Unity/Excel/Units.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectApopalypse\ProjectApopalypse_Unity\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22583F06-5F32-48FC-A5BB-50DB360C22C9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4CE35C-1AF4-46AA-81D5-F6BC149E804E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{3A2312A1-F630-46F4-AF7A-37D6220B2126}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="110">
   <si>
     <t>technicalName</t>
   </si>
@@ -249,9 +249,6 @@
     <t>passive4</t>
   </si>
   <si>
-    <t>defaultPassive</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -354,13 +351,10 @@
     <t>None</t>
   </si>
   <si>
-    <t>ehtan</t>
-  </si>
-  <si>
-    <t>EHTAN</t>
-  </si>
-  <si>
-    <t>iithishasjief Njeofjo</t>
+    <t>effectImpactTime</t>
+  </si>
+  <si>
+    <t>DefaultPassive</t>
   </si>
 </sst>
 </file>
@@ -410,7 +404,25 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="98">
+  <dxfs count="99">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2189,20 +2201,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C2383A53-3A2F-40EF-B721-6DA1839BF909}" name="Table1" displayName="Table1" ref="A1:CR4" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96">
-  <autoFilter ref="A1:CR4" xr:uid="{9EC39B5B-8F44-472E-918B-DBA77F12954E}"/>
-  <tableColumns count="96">
-    <tableColumn id="1" xr3:uid="{89B66E7D-F1B0-4F11-A8C4-437D2EE54D17}" name="technicalName" dataDxfId="95"/>
-    <tableColumn id="2" xr3:uid="{CC988DFD-F98F-486F-AD81-B53A776A7D5A}" name="displayName" dataDxfId="94"/>
-    <tableColumn id="3" xr3:uid="{44D15C63-6D62-495D-85F5-9CCF58B79FDE}" name="description" dataDxfId="93"/>
-    <tableColumn id="4" xr3:uid="{545FCCFA-9A67-4E7B-9071-9F021AE4B2AD}" name="rank" dataDxfId="92"/>
-    <tableColumn id="5" xr3:uid="{28D65B36-0E27-4A75-8220-E8BC8D82D324}" name="canMove" dataDxfId="91"/>
-    <tableColumn id="6" xr3:uid="{A42853E4-5F24-497D-870A-62AEF57FFEED}" name="canAttack" dataDxfId="90"/>
-    <tableColumn id="7" xr3:uid="{D2449210-25FD-4C20-88AB-9E6581657C27}" name="moveType" dataDxfId="89"/>
-    <tableColumn id="8" xr3:uid="{092C91A1-3DB7-4450-8F05-AAD1CDA0F14C}" name="targetAllies" dataDxfId="88"/>
-    <tableColumn id="9" xr3:uid="{8CE7E365-3646-4682-B988-BCD9972D5CE3}" name="targetEnemies" dataDxfId="87"/>
-    <tableColumn id="10" xr3:uid="{49914703-F632-4F6B-A5D7-AF9C3521999F}" name="splashOrigin" dataDxfId="86"/>
-    <tableColumn id="11" xr3:uid="{9CCCDE5D-9BBE-4F02-9B68-128D58CC29FE}" name="splashType" dataDxfId="85"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C2383A53-3A2F-40EF-B721-6DA1839BF909}" name="Table1" displayName="Table1" ref="A1:CS3" totalsRowShown="0" headerRowDxfId="98" dataDxfId="97">
+  <autoFilter ref="A1:CS3" xr:uid="{9EC39B5B-8F44-472E-918B-DBA77F12954E}"/>
+  <tableColumns count="97">
+    <tableColumn id="1" xr3:uid="{89B66E7D-F1B0-4F11-A8C4-437D2EE54D17}" name="technicalName" dataDxfId="96"/>
+    <tableColumn id="2" xr3:uid="{CC988DFD-F98F-486F-AD81-B53A776A7D5A}" name="displayName" dataDxfId="95"/>
+    <tableColumn id="3" xr3:uid="{44D15C63-6D62-495D-85F5-9CCF58B79FDE}" name="description" dataDxfId="94"/>
+    <tableColumn id="4" xr3:uid="{545FCCFA-9A67-4E7B-9071-9F021AE4B2AD}" name="rank" dataDxfId="93"/>
+    <tableColumn id="5" xr3:uid="{28D65B36-0E27-4A75-8220-E8BC8D82D324}" name="canMove" dataDxfId="92"/>
+    <tableColumn id="6" xr3:uid="{A42853E4-5F24-497D-870A-62AEF57FFEED}" name="canAttack" dataDxfId="91"/>
+    <tableColumn id="7" xr3:uid="{D2449210-25FD-4C20-88AB-9E6581657C27}" name="moveType" dataDxfId="90"/>
+    <tableColumn id="8" xr3:uid="{092C91A1-3DB7-4450-8F05-AAD1CDA0F14C}" name="targetAllies" dataDxfId="89"/>
+    <tableColumn id="9" xr3:uid="{8CE7E365-3646-4682-B988-BCD9972D5CE3}" name="targetEnemies" dataDxfId="88"/>
+    <tableColumn id="10" xr3:uid="{49914703-F632-4F6B-A5D7-AF9C3521999F}" name="splashOrigin" dataDxfId="87"/>
+    <tableColumn id="11" xr3:uid="{9CCCDE5D-9BBE-4F02-9B68-128D58CC29FE}" name="splashType" dataDxfId="86"/>
+    <tableColumn id="97" xr3:uid="{7C0F417B-4A77-4766-A004-0629EB93E7A9}" name="effectImpactTime" dataDxfId="85"/>
     <tableColumn id="12" xr3:uid="{A4D3FB9F-46F6-42E3-A00E-F3D2F6D4DB38}" name="passive1" dataDxfId="84"/>
     <tableColumn id="13" xr3:uid="{8385E9D4-FD43-4930-B457-432C24E6790C}" name="passive2" dataDxfId="83"/>
     <tableColumn id="14" xr3:uid="{1D9163BD-EEA7-4F85-9C91-2860370D68BC}" name="passive3" dataDxfId="82"/>
@@ -2590,10 +2603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66FF625-BC64-4C5F-8916-6942D597EF48}">
-  <dimension ref="A1:CR4"/>
+  <dimension ref="A1:CS3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="7.8" x14ac:dyDescent="0.15"/>
@@ -2603,92 +2616,92 @@
     <col min="3" max="8" width="8.77734375" style="1" customWidth="1"/>
     <col min="9" max="9" width="10.21875" style="1" customWidth="1"/>
     <col min="10" max="10" width="9.21875" style="1" customWidth="1"/>
-    <col min="11" max="15" width="8.77734375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="8.88671875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="10" style="1" customWidth="1"/>
-    <col min="18" max="18" width="9.6640625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="11.77734375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="10.21875" style="1" customWidth="1"/>
-    <col min="21" max="21" width="12.33203125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="12" style="1" customWidth="1"/>
-    <col min="23" max="23" width="14.109375" style="1" customWidth="1"/>
-    <col min="24" max="24" width="10.5546875" style="1" customWidth="1"/>
-    <col min="25" max="25" width="12.6640625" style="1" customWidth="1"/>
-    <col min="26" max="26" width="12.33203125" style="1" customWidth="1"/>
-    <col min="27" max="27" width="14.44140625" style="1" customWidth="1"/>
-    <col min="28" max="28" width="12.33203125" style="1" customWidth="1"/>
-    <col min="29" max="29" width="14.44140625" style="1" customWidth="1"/>
-    <col min="30" max="30" width="14.109375" style="1" customWidth="1"/>
-    <col min="31" max="31" width="16.21875" style="1" customWidth="1"/>
-    <col min="32" max="32" width="10.5546875" style="1" customWidth="1"/>
-    <col min="33" max="33" width="12.6640625" style="1" customWidth="1"/>
-    <col min="34" max="34" width="12.33203125" style="1" customWidth="1"/>
-    <col min="35" max="35" width="14.44140625" style="1" customWidth="1"/>
-    <col min="36" max="36" width="11.109375" style="1" customWidth="1"/>
-    <col min="37" max="37" width="13.21875" style="1" customWidth="1"/>
-    <col min="38" max="38" width="12.88671875" style="1" customWidth="1"/>
-    <col min="39" max="39" width="15" style="1" customWidth="1"/>
-    <col min="40" max="40" width="11.5546875" style="1" customWidth="1"/>
-    <col min="41" max="41" width="13.6640625" style="1" customWidth="1"/>
-    <col min="42" max="42" width="13.33203125" style="1" customWidth="1"/>
-    <col min="43" max="43" width="15.44140625" style="1" customWidth="1"/>
-    <col min="44" max="44" width="11.88671875" style="1" customWidth="1"/>
-    <col min="45" max="45" width="14" style="1" customWidth="1"/>
-    <col min="46" max="46" width="13.6640625" style="1" customWidth="1"/>
-    <col min="47" max="47" width="15.77734375" style="1" customWidth="1"/>
-    <col min="48" max="48" width="11.33203125" style="1" customWidth="1"/>
-    <col min="49" max="49" width="13.44140625" style="1" customWidth="1"/>
-    <col min="50" max="50" width="13.109375" style="1" customWidth="1"/>
-    <col min="51" max="51" width="15.21875" style="1" customWidth="1"/>
-    <col min="52" max="52" width="11.88671875" style="1" customWidth="1"/>
-    <col min="53" max="53" width="14" style="1" customWidth="1"/>
-    <col min="54" max="54" width="13.6640625" style="1" customWidth="1"/>
-    <col min="55" max="55" width="15.77734375" style="1" customWidth="1"/>
-    <col min="56" max="56" width="11.88671875" style="1" customWidth="1"/>
-    <col min="57" max="57" width="14" style="1" customWidth="1"/>
-    <col min="58" max="58" width="13.6640625" style="1" customWidth="1"/>
-    <col min="59" max="59" width="15.77734375" style="1" customWidth="1"/>
-    <col min="60" max="60" width="12.44140625" style="1" customWidth="1"/>
-    <col min="61" max="61" width="14.5546875" style="1" customWidth="1"/>
-    <col min="62" max="62" width="14.21875" style="1" customWidth="1"/>
-    <col min="63" max="63" width="16.33203125" style="1" customWidth="1"/>
-    <col min="64" max="64" width="9.6640625" style="1" customWidth="1"/>
-    <col min="65" max="65" width="11.77734375" style="1" customWidth="1"/>
-    <col min="66" max="66" width="11.44140625" style="1" customWidth="1"/>
-    <col min="67" max="67" width="13.5546875" style="1" customWidth="1"/>
-    <col min="68" max="68" width="10.77734375" style="1" customWidth="1"/>
-    <col min="69" max="69" width="12.88671875" style="1" customWidth="1"/>
-    <col min="70" max="70" width="12.5546875" style="1" customWidth="1"/>
-    <col min="71" max="71" width="14.6640625" style="1" customWidth="1"/>
-    <col min="72" max="72" width="11.6640625" style="1" customWidth="1"/>
-    <col min="73" max="73" width="13.77734375" style="1" customWidth="1"/>
-    <col min="74" max="74" width="13.44140625" style="1" customWidth="1"/>
-    <col min="75" max="75" width="15.5546875" style="1" customWidth="1"/>
-    <col min="76" max="76" width="8.88671875" style="1"/>
-    <col min="77" max="77" width="10.109375" style="1" customWidth="1"/>
-    <col min="78" max="78" width="9.77734375" style="1" customWidth="1"/>
-    <col min="79" max="79" width="11.88671875" style="1" customWidth="1"/>
-    <col min="80" max="80" width="10.77734375" style="1" customWidth="1"/>
-    <col min="81" max="81" width="12.88671875" style="1" customWidth="1"/>
-    <col min="82" max="82" width="12.5546875" style="1" customWidth="1"/>
-    <col min="83" max="83" width="14.6640625" style="1" customWidth="1"/>
-    <col min="84" max="84" width="8.88671875" style="1"/>
-    <col min="85" max="85" width="11" style="1" customWidth="1"/>
-    <col min="86" max="86" width="10.6640625" style="1" customWidth="1"/>
-    <col min="87" max="87" width="12.77734375" style="1" customWidth="1"/>
-    <col min="88" max="88" width="8.88671875" style="1"/>
-    <col min="89" max="89" width="9.5546875" style="1" customWidth="1"/>
-    <col min="90" max="90" width="9.21875" style="1" customWidth="1"/>
-    <col min="91" max="91" width="11.33203125" style="1" customWidth="1"/>
-    <col min="92" max="92" width="9.21875" style="1" customWidth="1"/>
-    <col min="93" max="93" width="8.88671875" style="1"/>
-    <col min="94" max="94" width="10.5546875" style="1" customWidth="1"/>
-    <col min="95" max="95" width="10.21875" style="1" customWidth="1"/>
-    <col min="96" max="96" width="12.33203125" style="1" customWidth="1"/>
-    <col min="97" max="16384" width="8.88671875" style="1"/>
+    <col min="11" max="16" width="8.77734375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="8.88671875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="10" style="1" customWidth="1"/>
+    <col min="19" max="19" width="9.6640625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="11.77734375" style="1" customWidth="1"/>
+    <col min="21" max="21" width="10.21875" style="1" customWidth="1"/>
+    <col min="22" max="22" width="12.33203125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="12" style="1" customWidth="1"/>
+    <col min="24" max="24" width="14.109375" style="1" customWidth="1"/>
+    <col min="25" max="25" width="10.5546875" style="1" customWidth="1"/>
+    <col min="26" max="26" width="12.6640625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="12.33203125" style="1" customWidth="1"/>
+    <col min="28" max="28" width="14.44140625" style="1" customWidth="1"/>
+    <col min="29" max="29" width="12.33203125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="14.44140625" style="1" customWidth="1"/>
+    <col min="31" max="31" width="14.109375" style="1" customWidth="1"/>
+    <col min="32" max="32" width="16.21875" style="1" customWidth="1"/>
+    <col min="33" max="33" width="10.5546875" style="1" customWidth="1"/>
+    <col min="34" max="34" width="12.6640625" style="1" customWidth="1"/>
+    <col min="35" max="35" width="12.33203125" style="1" customWidth="1"/>
+    <col min="36" max="36" width="14.44140625" style="1" customWidth="1"/>
+    <col min="37" max="37" width="11.109375" style="1" customWidth="1"/>
+    <col min="38" max="38" width="13.21875" style="1" customWidth="1"/>
+    <col min="39" max="39" width="12.88671875" style="1" customWidth="1"/>
+    <col min="40" max="40" width="15" style="1" customWidth="1"/>
+    <col min="41" max="41" width="11.5546875" style="1" customWidth="1"/>
+    <col min="42" max="42" width="13.6640625" style="1" customWidth="1"/>
+    <col min="43" max="43" width="13.33203125" style="1" customWidth="1"/>
+    <col min="44" max="44" width="15.44140625" style="1" customWidth="1"/>
+    <col min="45" max="45" width="11.88671875" style="1" customWidth="1"/>
+    <col min="46" max="46" width="14" style="1" customWidth="1"/>
+    <col min="47" max="47" width="13.6640625" style="1" customWidth="1"/>
+    <col min="48" max="48" width="15.77734375" style="1" customWidth="1"/>
+    <col min="49" max="49" width="11.33203125" style="1" customWidth="1"/>
+    <col min="50" max="50" width="13.44140625" style="1" customWidth="1"/>
+    <col min="51" max="51" width="13.109375" style="1" customWidth="1"/>
+    <col min="52" max="52" width="15.21875" style="1" customWidth="1"/>
+    <col min="53" max="53" width="11.88671875" style="1" customWidth="1"/>
+    <col min="54" max="54" width="14" style="1" customWidth="1"/>
+    <col min="55" max="55" width="13.6640625" style="1" customWidth="1"/>
+    <col min="56" max="56" width="15.77734375" style="1" customWidth="1"/>
+    <col min="57" max="57" width="11.88671875" style="1" customWidth="1"/>
+    <col min="58" max="58" width="14" style="1" customWidth="1"/>
+    <col min="59" max="59" width="13.6640625" style="1" customWidth="1"/>
+    <col min="60" max="60" width="15.77734375" style="1" customWidth="1"/>
+    <col min="61" max="61" width="12.44140625" style="1" customWidth="1"/>
+    <col min="62" max="62" width="14.5546875" style="1" customWidth="1"/>
+    <col min="63" max="63" width="14.21875" style="1" customWidth="1"/>
+    <col min="64" max="64" width="16.33203125" style="1" customWidth="1"/>
+    <col min="65" max="65" width="9.6640625" style="1" customWidth="1"/>
+    <col min="66" max="66" width="11.77734375" style="1" customWidth="1"/>
+    <col min="67" max="67" width="11.44140625" style="1" customWidth="1"/>
+    <col min="68" max="68" width="13.5546875" style="1" customWidth="1"/>
+    <col min="69" max="69" width="10.77734375" style="1" customWidth="1"/>
+    <col min="70" max="70" width="12.88671875" style="1" customWidth="1"/>
+    <col min="71" max="71" width="12.5546875" style="1" customWidth="1"/>
+    <col min="72" max="72" width="14.6640625" style="1" customWidth="1"/>
+    <col min="73" max="73" width="11.6640625" style="1" customWidth="1"/>
+    <col min="74" max="74" width="13.77734375" style="1" customWidth="1"/>
+    <col min="75" max="75" width="13.44140625" style="1" customWidth="1"/>
+    <col min="76" max="76" width="15.5546875" style="1" customWidth="1"/>
+    <col min="77" max="77" width="8.88671875" style="1"/>
+    <col min="78" max="78" width="10.109375" style="1" customWidth="1"/>
+    <col min="79" max="79" width="9.77734375" style="1" customWidth="1"/>
+    <col min="80" max="80" width="11.88671875" style="1" customWidth="1"/>
+    <col min="81" max="81" width="10.77734375" style="1" customWidth="1"/>
+    <col min="82" max="82" width="12.88671875" style="1" customWidth="1"/>
+    <col min="83" max="83" width="12.5546875" style="1" customWidth="1"/>
+    <col min="84" max="84" width="14.6640625" style="1" customWidth="1"/>
+    <col min="85" max="85" width="8.88671875" style="1"/>
+    <col min="86" max="86" width="11" style="1" customWidth="1"/>
+    <col min="87" max="87" width="10.6640625" style="1" customWidth="1"/>
+    <col min="88" max="88" width="12.77734375" style="1" customWidth="1"/>
+    <col min="89" max="89" width="8.88671875" style="1"/>
+    <col min="90" max="90" width="9.5546875" style="1" customWidth="1"/>
+    <col min="91" max="91" width="9.21875" style="1" customWidth="1"/>
+    <col min="92" max="92" width="11.33203125" style="1" customWidth="1"/>
+    <col min="93" max="93" width="9.21875" style="1" customWidth="1"/>
+    <col min="94" max="94" width="8.88671875" style="1"/>
+    <col min="95" max="95" width="10.5546875" style="1" customWidth="1"/>
+    <col min="96" max="96" width="10.21875" style="1" customWidth="1"/>
+    <col min="97" max="97" width="12.33203125" style="1" customWidth="1"/>
+    <col min="98" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:96" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:97" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2696,859 +2709,857 @@
         <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BS1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BT1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BU1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BW1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BX1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BY1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BZ1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="CA1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="CB1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="CC1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="CD1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="CE1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="CF1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="CG1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="CH1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="CI1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="CJ1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="CK1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="CL1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="CM1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="CN1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="CO1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="CP1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="CQ1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="CR1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="CS1" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:97" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="E2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="H2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L2" s="1">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>50</v>
+      </c>
+      <c r="R2" s="1">
+        <v>999</v>
+      </c>
+      <c r="S2" s="1">
+        <v>1</v>
+      </c>
+      <c r="T2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="U2" s="1">
+        <v>0</v>
+      </c>
+      <c r="V2" s="1">
+        <v>999</v>
+      </c>
+      <c r="W2" s="1">
+        <v>1</v>
+      </c>
+      <c r="X2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>999</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>999</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>999</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="1">
+        <v>999</v>
+      </c>
+      <c r="AM2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AP2" s="1">
+        <v>999</v>
+      </c>
+      <c r="AQ2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT2" s="1">
+        <v>999</v>
+      </c>
+      <c r="AU2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AV2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AW2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX2" s="1">
+        <v>999</v>
+      </c>
+      <c r="AY2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AZ2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BA2" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB2" s="1">
+        <v>999</v>
+      </c>
+      <c r="BC2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BD2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BE2" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF2" s="1">
+        <v>999</v>
+      </c>
+      <c r="BG2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BI2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ2" s="1">
+        <v>999</v>
+      </c>
+      <c r="BK2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BL2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BM2" s="1">
+        <v>2</v>
+      </c>
+      <c r="BN2" s="1">
+        <v>999</v>
+      </c>
+      <c r="BO2" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="BP2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BQ2" s="1">
+        <v>0</v>
+      </c>
+      <c r="BR2" s="1">
+        <v>999</v>
+      </c>
+      <c r="BS2" s="1">
+        <v>0</v>
+      </c>
+      <c r="BT2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BU2" s="1">
+        <v>5</v>
+      </c>
+      <c r="BV2" s="1">
+        <v>999</v>
+      </c>
+      <c r="BW2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BX2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BY2" s="1">
+        <v>2</v>
+      </c>
+      <c r="BZ2" s="1">
+        <v>999</v>
+      </c>
+      <c r="CA2" s="1">
+        <v>1</v>
+      </c>
+      <c r="CB2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="CC2" s="1">
+        <v>5</v>
+      </c>
+      <c r="CD2" s="1">
+        <v>999</v>
+      </c>
+      <c r="CE2" s="1">
+        <v>1</v>
+      </c>
+      <c r="CF2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="CG2" s="1">
+        <v>1</v>
+      </c>
+      <c r="CH2" s="1">
+        <v>999</v>
+      </c>
+      <c r="CI2" s="1">
+        <v>1</v>
+      </c>
+      <c r="CJ2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="CK2" s="1">
+        <v>0</v>
+      </c>
+      <c r="CL2" s="1">
+        <v>999</v>
+      </c>
+      <c r="CM2" s="1">
+        <v>1</v>
+      </c>
+      <c r="CN2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="CO2" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="CP2" s="1">
+        <v>1</v>
+      </c>
+      <c r="CQ2" s="1">
+        <v>10</v>
+      </c>
+      <c r="CR2" s="1">
+        <v>1</v>
+      </c>
+      <c r="CS2" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:97" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB1" s="1" t="s">
+      <c r="K3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="L3" s="1">
+        <v>2</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>50</v>
+      </c>
+      <c r="R3" s="1">
+        <v>999</v>
+      </c>
+      <c r="S3" s="1">
+        <v>1</v>
+      </c>
+      <c r="T3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="U3" s="1">
+        <v>0</v>
+      </c>
+      <c r="V3" s="1">
+        <v>999</v>
+      </c>
+      <c r="W3" s="1">
+        <v>1</v>
+      </c>
+      <c r="X3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>999</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>999</v>
+      </c>
+      <c r="AE3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="1">
+        <v>999</v>
+      </c>
+      <c r="AI3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="1">
+        <v>999</v>
+      </c>
+      <c r="AM3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AP3" s="1">
+        <v>999</v>
+      </c>
+      <c r="AQ3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT3" s="1">
+        <v>999</v>
+      </c>
+      <c r="AU3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AV3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AW3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX3" s="1">
+        <v>999</v>
+      </c>
+      <c r="AY3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AZ3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BA3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB3" s="1">
+        <v>999</v>
+      </c>
+      <c r="BC3" s="1">
+        <v>1</v>
+      </c>
+      <c r="BD3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BE3" s="1">
+        <v>1</v>
+      </c>
+      <c r="BF3" s="1">
+        <v>999</v>
+      </c>
+      <c r="BG3" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BI3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ3" s="1">
+        <v>999</v>
+      </c>
+      <c r="BK3" s="1">
+        <v>1</v>
+      </c>
+      <c r="BL3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BM3" s="1">
+        <v>2</v>
+      </c>
+      <c r="BN3" s="1">
+        <v>999</v>
+      </c>
+      <c r="BO3" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="BP3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BQ3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BR3" s="1">
+        <v>999</v>
+      </c>
+      <c r="BS3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BT3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BU3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BV3" s="1">
+        <v>999</v>
+      </c>
+      <c r="BW3" s="1">
+        <v>1</v>
+      </c>
+      <c r="BX3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="BY3" s="1">
+        <v>2</v>
+      </c>
+      <c r="BZ3" s="1">
+        <v>999</v>
+      </c>
+      <c r="CA3" s="1">
+        <v>1</v>
+      </c>
+      <c r="CB3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="CC3" s="1">
         <v>5</v>
       </c>
-      <c r="AC1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="CD3" s="1">
+        <v>999</v>
+      </c>
+      <c r="CE3" s="1">
+        <v>1</v>
+      </c>
+      <c r="CF3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="CG3" s="1">
+        <v>1</v>
+      </c>
+      <c r="CH3" s="1">
+        <v>999</v>
+      </c>
+      <c r="CI3" s="1">
+        <v>1</v>
+      </c>
+      <c r="CJ3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="CK3" s="1">
+        <v>0</v>
+      </c>
+      <c r="CL3" s="1">
+        <v>999</v>
+      </c>
+      <c r="CM3" s="1">
+        <v>1</v>
+      </c>
+      <c r="CN3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="CO3" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="CP3" s="1">
+        <v>1</v>
+      </c>
+      <c r="CQ3" s="1">
         <v>10</v>
       </c>
-      <c r="BA1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="BB1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="BD1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="BE1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="BF1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="BG1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="BH1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="BI1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="BJ1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="BK1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="BL1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="BM1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="BN1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="BO1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="BP1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="BQ1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="BR1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="BS1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="BT1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="BU1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="BV1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="BW1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="BX1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BY1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="BZ1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="CA1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="CB1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="CC1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="CD1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="CE1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="CF1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="CG1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="CH1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="CI1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="CJ1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="CK1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="CL1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="CM1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="CN1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="CO1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="CP1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="CQ1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="CR1" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:96" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="P2" s="1">
-        <v>50</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>999</v>
-      </c>
-      <c r="R2" s="1">
-        <v>1</v>
-      </c>
-      <c r="S2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="T2" s="1">
-        <v>0</v>
-      </c>
-      <c r="U2" s="1">
-        <v>999</v>
-      </c>
-      <c r="V2" s="1">
-        <v>1</v>
-      </c>
-      <c r="W2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="X2" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="1">
-        <v>999</v>
-      </c>
-      <c r="Z2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="1">
-        <v>999</v>
-      </c>
-      <c r="AD2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="AF2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AG2" s="1">
-        <v>999</v>
-      </c>
-      <c r="AH2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="AJ2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AK2" s="1">
-        <v>999</v>
-      </c>
-      <c r="AL2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AM2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AO2" s="1">
-        <v>999</v>
-      </c>
-      <c r="AP2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AQ2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="AR2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AS2" s="1">
-        <v>999</v>
-      </c>
-      <c r="AT2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AU2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="AV2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AW2" s="1">
-        <v>999</v>
-      </c>
-      <c r="AX2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AY2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="AZ2" s="1">
-        <v>0</v>
-      </c>
-      <c r="BA2" s="1">
-        <v>999</v>
-      </c>
-      <c r="BB2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BC2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="BD2" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE2" s="1">
-        <v>999</v>
-      </c>
-      <c r="BF2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BG2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="BH2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BI2" s="1">
-        <v>999</v>
-      </c>
-      <c r="BJ2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BK2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="BL2" s="1">
-        <v>2</v>
-      </c>
-      <c r="BM2" s="1">
-        <v>999</v>
-      </c>
-      <c r="BN2" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="BO2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="BP2" s="1">
-        <v>0</v>
-      </c>
-      <c r="BQ2" s="1">
-        <v>999</v>
-      </c>
-      <c r="BR2" s="1">
-        <v>0</v>
-      </c>
-      <c r="BS2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="BT2" s="1">
-        <v>5</v>
-      </c>
-      <c r="BU2" s="1">
-        <v>999</v>
-      </c>
-      <c r="BV2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BW2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="BX2" s="1">
-        <v>2</v>
-      </c>
-      <c r="BY2" s="1">
-        <v>999</v>
-      </c>
-      <c r="BZ2" s="1">
-        <v>1</v>
-      </c>
-      <c r="CA2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="CB2" s="1">
-        <v>5</v>
-      </c>
-      <c r="CC2" s="1">
-        <v>999</v>
-      </c>
-      <c r="CD2" s="1">
-        <v>1</v>
-      </c>
-      <c r="CE2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="CF2" s="1">
-        <v>1</v>
-      </c>
-      <c r="CG2" s="1">
-        <v>999</v>
-      </c>
-      <c r="CH2" s="1">
-        <v>1</v>
-      </c>
-      <c r="CI2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="CJ2" s="1">
-        <v>0</v>
-      </c>
-      <c r="CK2" s="1">
-        <v>999</v>
-      </c>
-      <c r="CL2" s="1">
-        <v>1</v>
-      </c>
-      <c r="CM2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="CN2" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="CO2" s="1">
-        <v>1</v>
-      </c>
-      <c r="CP2" s="1">
-        <v>10</v>
-      </c>
-      <c r="CQ2" s="1">
-        <v>1</v>
-      </c>
-      <c r="CR2" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:96" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E3" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="H3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="P3" s="1">
-        <v>50</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>999</v>
-      </c>
-      <c r="R3" s="1">
-        <v>1</v>
-      </c>
-      <c r="S3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="T3" s="1">
-        <v>0</v>
-      </c>
-      <c r="U3" s="1">
-        <v>999</v>
-      </c>
-      <c r="V3" s="1">
-        <v>1</v>
-      </c>
-      <c r="W3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="X3" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="1">
-        <v>999</v>
-      </c>
-      <c r="Z3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="1">
-        <v>999</v>
-      </c>
-      <c r="AD3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="AF3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="1">
-        <v>999</v>
-      </c>
-      <c r="AH3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AI3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="AJ3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AK3" s="1">
-        <v>999</v>
-      </c>
-      <c r="AL3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AM3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AO3" s="1">
-        <v>999</v>
-      </c>
-      <c r="AP3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AQ3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="AR3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AS3" s="1">
-        <v>999</v>
-      </c>
-      <c r="AT3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AU3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="AV3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AW3" s="1">
-        <v>999</v>
-      </c>
-      <c r="AX3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AY3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="AZ3" s="1">
-        <v>0</v>
-      </c>
-      <c r="BA3" s="1">
-        <v>999</v>
-      </c>
-      <c r="BB3" s="1">
-        <v>1</v>
-      </c>
-      <c r="BC3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="BD3" s="1">
-        <v>1</v>
-      </c>
-      <c r="BE3" s="1">
-        <v>999</v>
-      </c>
-      <c r="BF3" s="1">
-        <v>1</v>
-      </c>
-      <c r="BG3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="BH3" s="1">
-        <v>0</v>
-      </c>
-      <c r="BI3" s="1">
-        <v>999</v>
-      </c>
-      <c r="BJ3" s="1">
-        <v>1</v>
-      </c>
-      <c r="BK3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="BL3" s="1">
-        <v>2</v>
-      </c>
-      <c r="BM3" s="1">
-        <v>999</v>
-      </c>
-      <c r="BN3" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="BO3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="BP3" s="1">
-        <v>0</v>
-      </c>
-      <c r="BQ3" s="1">
-        <v>999</v>
-      </c>
-      <c r="BR3" s="1">
-        <v>0</v>
-      </c>
-      <c r="BS3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="BT3" s="1">
-        <v>0</v>
-      </c>
-      <c r="BU3" s="1">
-        <v>999</v>
-      </c>
-      <c r="BV3" s="1">
-        <v>1</v>
-      </c>
-      <c r="BW3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="BX3" s="1">
-        <v>2</v>
-      </c>
-      <c r="BY3" s="1">
-        <v>999</v>
-      </c>
-      <c r="BZ3" s="1">
-        <v>1</v>
-      </c>
-      <c r="CA3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="CB3" s="1">
-        <v>5</v>
-      </c>
-      <c r="CC3" s="1">
-        <v>999</v>
-      </c>
-      <c r="CD3" s="1">
-        <v>1</v>
-      </c>
-      <c r="CE3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="CF3" s="1">
-        <v>1</v>
-      </c>
-      <c r="CG3" s="1">
-        <v>999</v>
-      </c>
-      <c r="CH3" s="1">
-        <v>1</v>
-      </c>
-      <c r="CI3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="CJ3" s="1">
-        <v>0</v>
-      </c>
-      <c r="CK3" s="1">
-        <v>999</v>
-      </c>
-      <c r="CL3" s="1">
-        <v>1</v>
-      </c>
-      <c r="CM3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="CN3" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="CO3" s="1">
-        <v>1</v>
-      </c>
-      <c r="CP3" s="1">
-        <v>10</v>
-      </c>
-      <c r="CQ3" s="1">
-        <v>1</v>
-      </c>
-      <c r="CR3" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:96" x14ac:dyDescent="0.15">
-      <c r="A4" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>111</v>
+      <c r="CR3" s="1">
+        <v>1</v>
+      </c>
+      <c r="CS3" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>